<commit_message>
Corrected code of Parser
</commit_message>
<xml_diff>
--- a/bin/Parse Table.xlsx
+++ b/bin/Parse Table.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="58">
   <si>
     <t>id</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>S32</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>S34</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>S36</t>
   </si>
 </sst>
 </file>
@@ -514,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V34"/>
+  <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -701,6 +713,9 @@
       <c r="B9" t="s">
         <v>24</v>
       </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
       <c r="S9">
         <v>9</v>
       </c>
@@ -839,8 +854,14 @@
       <c r="A18">
         <v>16</v>
       </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
       <c r="T18">
         <v>24</v>
+      </c>
+      <c r="U18">
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -851,7 +872,7 @@
         <v>27</v>
       </c>
       <c r="U19">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -993,7 +1014,7 @@
         <v>39</v>
       </c>
       <c r="N27" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -1078,7 +1099,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:21">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1088,11 +1109,14 @@
       <c r="D33" t="s">
         <v>29</v>
       </c>
+      <c r="I33" t="s">
+        <v>29</v>
+      </c>
       <c r="M33" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:21">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1107,6 +1131,74 @@
       </c>
       <c r="M34" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35">
+        <v>33</v>
+      </c>
+      <c r="I35" t="s">
+        <v>54</v>
+      </c>
+      <c r="M35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21">
+      <c r="A36">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" t="s">
+        <v>55</v>
+      </c>
+      <c r="S36">
+        <v>35</v>
+      </c>
+      <c r="T36">
+        <v>10</v>
+      </c>
+      <c r="U36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="A37">
+        <v>35</v>
+      </c>
+      <c r="F37" t="s">
+        <v>57</v>
+      </c>
+      <c r="H37" t="s">
+        <v>49</v>
+      </c>
+      <c r="J37" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21">
+      <c r="A38">
+        <v>36</v>
+      </c>
+      <c r="F38" t="s">
+        <v>56</v>
+      </c>
+      <c r="H38" t="s">
+        <v>56</v>
+      </c>
+      <c r="J38" t="s">
+        <v>56</v>
+      </c>
+      <c r="K38" t="s">
+        <v>56</v>
+      </c>
+      <c r="L38" t="s">
+        <v>56</v>
+      </c>
+      <c r="N38" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>